<commit_message>
Archives of past results
</commit_message>
<xml_diff>
--- a/Chapter1/data/DredgeResults.xlsx
+++ b/Chapter1/data/DredgeResults.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\shinycrab\Chapter1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB21B14-0762-426E-8867-0737C2332DC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6F454E-AC9F-4B1B-840E-C6056102A407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{AB9D09A7-83A1-4A69-B86C-3C8B58B59AF9}"/>
+    <workbookView xWindow="-19320" yWindow="270" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="4" xr2:uid="{AB9D09A7-83A1-4A69-B86C-3C8B58B59AF9}"/>
   </bookViews>
   <sheets>
     <sheet name="B90~SumLandings" sheetId="1" r:id="rId1"/>
     <sheet name="B90~LandingsCPUE" sheetId="2" r:id="rId2"/>
     <sheet name="T38~SumLandings" sheetId="3" r:id="rId3"/>
     <sheet name="T38~LandingsCPUE" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="TotalCPUE~Landings" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
   <si>
     <t>CPUE</t>
   </si>
@@ -118,52 +118,46 @@
     <t>Sublegal LAG</t>
   </si>
   <si>
-    <t>Credits</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Pub Pol</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Orient</t>
-  </si>
-  <si>
-    <t>Soc. Science</t>
-  </si>
-  <si>
-    <t>Fisheries</t>
-  </si>
-  <si>
-    <t>B+</t>
-  </si>
-  <si>
-    <t>Econ</t>
-  </si>
-  <si>
-    <t>Env. Bio</t>
-  </si>
-  <si>
-    <t>Biometry</t>
-  </si>
-  <si>
-    <t>Quant</t>
-  </si>
-  <si>
-    <t>Ecosytem</t>
-  </si>
-  <si>
-    <t>Grade Points</t>
-  </si>
-  <si>
-    <t>Sum Points</t>
+    <t>E98</t>
+  </si>
+  <si>
+    <t>E99</t>
+  </si>
+  <si>
+    <t>P88</t>
+  </si>
+  <si>
+    <t>T06</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>Independents</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r2 adj</t>
+  </si>
+  <si>
+    <t>F stat</t>
+  </si>
+  <si>
+    <t>w/ lag</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B90 (1980)</t>
+  </si>
+  <si>
+    <t>B90 (2003)</t>
   </si>
 </sst>
 </file>
@@ -2046,309 +2040,86 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE732D2-06B7-4898-950B-CEFB4C8A7074}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>10</v>
-      </c>
-      <c r="B1">
-        <v>10</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>5.6750000000000002E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.32329999999999998</v>
+      </c>
+      <c r="D2">
+        <v>0.2712</v>
+      </c>
+      <c r="E2">
+        <v>6.2110000000000003</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <f>H2/3</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">H3/3</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>9.9</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>3.3000000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>95.1</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>9.9</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>3.3000000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-      <c r="I8">
-        <f>H8/4</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9">
-        <v>12</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10">
-        <v>12</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11">
-        <v>12</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>135</v>
-      </c>
-      <c r="B12">
-        <v>150</v>
-      </c>
-      <c r="I12">
-        <f>AVERAGE(I2:I11)</f>
-        <v>3.8600000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>SUM(A1:A13)</f>
-        <v>439.1</v>
-      </c>
-      <c r="B14">
-        <f>SUM(B1:B13)</f>
-        <v>466</v>
-      </c>
-      <c r="C14">
-        <f>A14/B14</f>
-        <v>0.94227467811158805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>